<commit_message>
Slight base code refactor Added initial StoreItem models and deserialization algorithms
</commit_message>
<xml_diff>
--- a/vfBattleTechMod-ProcGenStores/Res/xlrp-store-content.xlsx
+++ b/vfBattleTechMod-ProcGenStores/Res/xlrp-store-content.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen Weistra\gitrepos\vfBattleTechMod-Core\vfBattleTechMod-ProcGenStores\Res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D603D143-A40B-473E-ADC0-9BC8A9753440}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9429820A-E639-4A2B-B293-F48519C1E35E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4275" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4275" yWindow="-21720" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="6" r:id="rId1"/>
@@ -20,12 +20,12 @@
     <sheet name="JumpJetDef" sheetId="4" r:id="rId5"/>
     <sheet name="WeaponDef" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="619">
   <si>
     <t>ActuatorTemplate</t>
   </si>
@@ -1665,36 +1665,18 @@
     <t>Id</t>
   </si>
   <si>
-    <t>Prototype date (Faction)</t>
-  </si>
-  <si>
-    <t>Production Date (Faction)</t>
-  </si>
-  <si>
     <t>Common Date</t>
   </si>
   <si>
     <t>Extinction Date</t>
   </si>
   <si>
-    <t>2559 (TH)</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
     <t>Availability</t>
   </si>
   <si>
-    <t>2567 (TH)</t>
-  </si>
-  <si>
-    <t>3040 (FS)</t>
-  </si>
-  <si>
-    <t>Reintro (Faction)</t>
-  </si>
-  <si>
     <t>Rare</t>
   </si>
   <si>
@@ -1725,21 +1707,6 @@
     <t>Availability Scale</t>
   </si>
   <si>
-    <t>2556 (TH)</t>
-  </si>
-  <si>
-    <t>2579 (TH)</t>
-  </si>
-  <si>
-    <t>3035 (LC)</t>
-  </si>
-  <si>
-    <t>3065 (LC)</t>
-  </si>
-  <si>
-    <t>3068 (LC)</t>
-  </si>
-  <si>
     <t>Inner Sphere Faction Codes</t>
   </si>
   <si>
@@ -1879,6 +1846,42 @@
   </si>
   <si>
     <t>Faction specific</t>
+  </si>
+  <si>
+    <t>3065|LC</t>
+  </si>
+  <si>
+    <t>Prototype date|Faction</t>
+  </si>
+  <si>
+    <t>Production Date|Faction</t>
+  </si>
+  <si>
+    <t>Reintro|Faction</t>
+  </si>
+  <si>
+    <t>3068|LC</t>
+  </si>
+  <si>
+    <t>2556|TH</t>
+  </si>
+  <si>
+    <t>2579|TH</t>
+  </si>
+  <si>
+    <t>3035|LC</t>
+  </si>
+  <si>
+    <t>2559|TH</t>
+  </si>
+  <si>
+    <t>2567|TH</t>
+  </si>
+  <si>
+    <t>3040|FS</t>
+  </si>
+  <si>
+    <t>Should Never Appear, like ever. Set to ubiquitous for testing purposes…</t>
   </si>
 </sst>
 </file>
@@ -2346,8 +2349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0111B82B-1818-471F-9FB0-9DF983CFAC3B}">
   <dimension ref="B1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2361,252 +2364,253 @@
     <row r="1" spans="2:6" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:6" ht="15.75" thickBot="1">
       <c r="B2" s="6" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>594</v>
+        <v>583</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>608</v>
+        <v>597</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>594</v>
+        <v>583</v>
       </c>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="5" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>595</v>
+        <v>584</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>605</v>
+        <v>594</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>610</v>
+        <v>599</v>
       </c>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="3" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>596</v>
+        <v>585</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>606</v>
+        <v>595</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>611</v>
+        <v>600</v>
       </c>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" s="3" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>597</v>
+        <v>586</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>607</v>
+        <v>596</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>612</v>
+        <v>601</v>
       </c>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>587</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>598</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>609</v>
-      </c>
       <c r="F6" s="14" t="s">
-        <v>615</v>
+        <v>604</v>
       </c>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="3" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>599</v>
+        <v>588</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>616</v>
+        <v>605</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>617</v>
+        <v>606</v>
       </c>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="3" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>600</v>
+        <v>589</v>
       </c>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="3" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>601</v>
+        <v>590</v>
       </c>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="3" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>602</v>
+        <v>591</v>
       </c>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="3" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>603</v>
+        <v>592</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="15.75" thickBot="1">
       <c r="B12" s="4" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>604</v>
+        <v>593</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="15.75" thickBot="1"/>
     <row r="14" spans="2:6" ht="15.75" thickBot="1">
       <c r="B14" s="9" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>614</v>
+        <v>603</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="30">
       <c r="B15" s="10" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>613</v>
+        <v>602</v>
       </c>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="11" t="s">
-        <v>573</v>
+        <v>562</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="12" t="s">
-        <v>574</v>
+        <v>563</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="12" t="s">
-        <v>575</v>
+        <v>564</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" s="12" t="s">
-        <v>576</v>
+        <v>565</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" s="11" t="s">
-        <v>577</v>
+        <v>566</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="30">
       <c r="B21" s="12" t="s">
-        <v>578</v>
+        <v>567</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" s="12" t="s">
-        <v>579</v>
+        <v>568</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" s="12" t="s">
-        <v>580</v>
+        <v>569</v>
       </c>
     </row>
     <row r="24" spans="2:2" ht="30">
       <c r="B24" s="12" t="s">
-        <v>581</v>
+        <v>570</v>
       </c>
     </row>
     <row r="25" spans="2:2" ht="30">
       <c r="B25" s="12" t="s">
-        <v>582</v>
+        <v>571</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" s="12" t="s">
-        <v>583</v>
+        <v>572</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" s="12" t="s">
-        <v>584</v>
+        <v>573</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" s="12" t="s">
-        <v>585</v>
+        <v>574</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" s="12" t="s">
-        <v>586</v>
+        <v>575</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" s="12" t="s">
-        <v>587</v>
+        <v>576</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" s="7" t="s">
-        <v>588</v>
+        <v>577</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" s="7" t="s">
-        <v>589</v>
+        <v>578</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" s="7" t="s">
-        <v>590</v>
+        <v>579</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" s="7" t="s">
-        <v>591</v>
+        <v>580</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" s="7" t="s">
-        <v>592</v>
+        <v>581</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="15.75" thickBot="1">
       <c r="B36" s="8" t="s">
-        <v>593</v>
+        <v>582</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3603,11 +3607,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G105"/>
+  <dimension ref="A1:H105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomLeft" activeCell="H92" sqref="H92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3621,372 +3625,375 @@
     <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>545</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>555</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>191</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>192</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>193</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>194</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>195</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>196</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>197</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>198</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>199</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>200</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>201</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>202</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>203</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>204</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>205</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -3994,22 +4001,22 @@
         <v>206</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -4017,22 +4024,22 @@
         <v>207</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -4040,22 +4047,22 @@
         <v>208</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -4063,22 +4070,22 @@
         <v>209</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -4086,22 +4093,22 @@
         <v>210</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -4109,22 +4116,22 @@
         <v>211</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -4132,22 +4139,22 @@
         <v>212</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -4155,22 +4162,22 @@
         <v>213</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -4178,22 +4185,22 @@
         <v>214</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -4201,22 +4208,22 @@
         <v>215</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -4224,22 +4231,22 @@
         <v>216</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -4247,22 +4254,22 @@
         <v>217</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -4270,22 +4277,22 @@
         <v>218</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -4293,22 +4300,22 @@
         <v>219</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -4316,22 +4323,22 @@
         <v>220</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -4339,22 +4346,22 @@
         <v>221</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -4362,22 +4369,22 @@
         <v>222</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -4385,22 +4392,22 @@
         <v>223</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -4408,22 +4415,22 @@
         <v>224</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -4431,22 +4438,22 @@
         <v>225</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -4454,22 +4461,22 @@
         <v>226</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -4477,22 +4484,22 @@
         <v>227</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -4500,22 +4507,22 @@
         <v>228</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -4523,22 +4530,22 @@
         <v>229</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -4546,22 +4553,22 @@
         <v>230</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -4569,22 +4576,22 @@
         <v>231</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -4592,22 +4599,22 @@
         <v>232</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -4615,22 +4622,22 @@
         <v>233</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -4638,22 +4645,22 @@
         <v>234</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -4661,22 +4668,22 @@
         <v>235</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -4684,22 +4691,22 @@
         <v>236</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -4707,22 +4714,22 @@
         <v>237</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -4730,22 +4737,22 @@
         <v>238</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -4753,22 +4760,22 @@
         <v>239</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -4776,22 +4783,22 @@
         <v>240</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -4799,22 +4806,22 @@
         <v>241</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -4822,22 +4829,22 @@
         <v>242</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -4845,22 +4852,22 @@
         <v>243</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -4868,22 +4875,22 @@
         <v>244</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -4891,22 +4898,22 @@
         <v>245</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -4914,22 +4921,22 @@
         <v>246</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -4937,22 +4944,22 @@
         <v>247</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -4960,22 +4967,22 @@
         <v>248</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -4983,22 +4990,22 @@
         <v>249</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -5006,22 +5013,22 @@
         <v>250</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -5029,22 +5036,22 @@
         <v>251</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -5052,22 +5059,22 @@
         <v>252</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -5075,22 +5082,22 @@
         <v>253</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -5098,22 +5105,22 @@
         <v>254</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -5121,22 +5128,22 @@
         <v>255</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -5144,22 +5151,22 @@
         <v>256</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -5167,22 +5174,22 @@
         <v>257</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -5190,22 +5197,22 @@
         <v>258</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -5213,22 +5220,22 @@
         <v>259</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -5236,22 +5243,22 @@
         <v>260</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -5259,22 +5266,22 @@
         <v>261</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -5282,22 +5289,22 @@
         <v>262</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -5305,22 +5312,22 @@
         <v>263</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -5328,22 +5335,22 @@
         <v>264</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -5351,22 +5358,22 @@
         <v>265</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -5374,22 +5381,22 @@
         <v>266</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -5397,22 +5404,22 @@
         <v>267</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -5420,22 +5427,22 @@
         <v>268</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -5443,390 +5450,393 @@
         <v>269</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
       <c r="A81" t="s">
         <v>270</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
       <c r="A82" t="s">
         <v>271</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
       <c r="A83" t="s">
         <v>272</v>
       </c>
       <c r="B83" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="G83" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="C83" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="G83" s="2" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7">
+    </row>
+    <row r="84" spans="1:8">
       <c r="A84" t="s">
         <v>273</v>
       </c>
       <c r="B84" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="G84" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="C84" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="F84" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="G84" s="2" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7">
+    </row>
+    <row r="85" spans="1:8">
       <c r="A85" t="s">
         <v>274</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
       <c r="A86" t="s">
         <v>275</v>
       </c>
       <c r="B86" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="G86" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="C86" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7">
+    </row>
+    <row r="87" spans="1:8">
       <c r="A87" t="s">
         <v>276</v>
       </c>
       <c r="B87" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="G87" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="C87" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="G87" s="2" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7">
+    </row>
+    <row r="88" spans="1:8">
       <c r="A88" t="s">
         <v>277</v>
       </c>
       <c r="B88" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="G88" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="C88" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="G88" s="2" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7">
+    </row>
+    <row r="89" spans="1:8">
       <c r="A89" t="s">
         <v>278</v>
       </c>
       <c r="B89" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="G89" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="C89" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="E89" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="G89" s="2" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7">
+    </row>
+    <row r="90" spans="1:8">
       <c r="A90" t="s">
         <v>279</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
       <c r="A91" t="s">
         <v>280</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>569</v>
+        <v>607</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>570</v>
+        <v>611</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F91">
         <v>3072</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7">
+        <v>552</v>
+      </c>
+      <c r="H91" s="2" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8">
       <c r="A92" t="s">
         <v>281</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8">
       <c r="A93" t="s">
         <v>282</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8">
       <c r="A94" t="s">
         <v>283</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>566</v>
+        <v>612</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>567</v>
+        <v>613</v>
       </c>
       <c r="D94">
         <v>2865</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>568</v>
+        <v>614</v>
       </c>
       <c r="F94">
         <v>3045</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8">
       <c r="A95" t="s">
         <v>284</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>550</v>
+        <v>615</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>553</v>
+        <v>616</v>
       </c>
       <c r="D95">
         <v>2865</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>554</v>
+        <v>617</v>
       </c>
       <c r="F95">
         <v>3045</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8">
       <c r="A96" t="s">
         <v>285</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -5834,22 +5844,22 @@
         <v>286</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -5857,22 +5867,22 @@
         <v>287</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>550</v>
+        <v>615</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>553</v>
+        <v>616</v>
       </c>
       <c r="D98">
         <v>2865</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>554</v>
+        <v>617</v>
       </c>
       <c r="F98">
         <v>3045</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -5880,22 +5890,22 @@
         <v>288</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -5903,22 +5913,22 @@
         <v>289</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -5926,22 +5936,22 @@
         <v>290</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -5949,22 +5959,22 @@
         <v>291</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -5972,22 +5982,22 @@
         <v>292</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -5995,22 +6005,22 @@
         <v>293</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -6018,22 +6028,22 @@
         <v>294</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
   </sheetData>

</xml_diff>